<commit_message>
change duplicate person name record in example xlsx file
</commit_message>
<xml_diff>
--- a/backend/resources/example.xlsx
+++ b/backend/resources/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soamid\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\OneDrive\Pulpit\Studia\SEMESTR 5\TECHNOLOGIE OBIEKTOWE\mi-pt-1300-majestatycznebestie\backend\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B8F606FC-8ED6-4013-94C9-E5EB03B1BF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A737DDF9-F8C7-465B-972B-ABBFEC02D19D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6756D010-450D-4BFD-A75E-591CA2C92982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="464">
   <si>
     <t>ID</t>
   </si>
@@ -1425,6 +1425,9 @@
   </si>
   <si>
     <t>żebrak</t>
+  </si>
+  <si>
+    <t>idzik</t>
   </si>
 </sst>
 </file>
@@ -1434,7 +1437,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1478,8 +1481,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="19">
     <dxf>
@@ -1882,18 +1885,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="I37" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" customWidth="1"/>
     <col min="12" max="19" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1952,7 +1955,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>15</v>
       </c>
@@ -1990,7 +1993,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>65</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>135</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>125</v>
       </c>
@@ -2104,7 +2107,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>127</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>105</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>110</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>151</v>
       </c>
@@ -2256,7 +2259,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>140</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>83</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>169</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>82</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>26</v>
       </c>
@@ -2446,7 +2449,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43</v>
       </c>
@@ -2484,7 +2487,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>29</v>
       </c>
@@ -2522,7 +2525,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>35</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>38</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>170</v>
       </c>
@@ -2636,7 +2639,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>139</v>
       </c>
@@ -2674,7 +2677,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>74</v>
       </c>
@@ -2712,7 +2715,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>167</v>
       </c>
@@ -2750,7 +2753,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>88</v>
       </c>
@@ -2788,7 +2791,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>175</v>
       </c>
@@ -2826,7 +2829,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>132</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>142</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>100</v>
       </c>
@@ -2940,7 +2943,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2978,7 +2981,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8</v>
       </c>
@@ -3016,7 +3019,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>59</v>
       </c>
@@ -3054,7 +3057,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>31</v>
       </c>
@@ -3092,7 +3095,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>121</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>49</v>
       </c>
@@ -3168,7 +3171,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>130</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>160</v>
       </c>
@@ -3244,7 +3247,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>113</v>
       </c>
@@ -3282,7 +3285,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>120</v>
       </c>
@@ -3320,7 +3323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>25</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>168</v>
       </c>
@@ -3396,7 +3399,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>53</v>
       </c>
@@ -3434,7 +3437,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>47</v>
       </c>
@@ -3472,7 +3475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>137</v>
       </c>
@@ -3510,7 +3513,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>138</v>
       </c>
@@ -3548,7 +3551,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3586,7 +3589,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>13</v>
       </c>
@@ -3624,7 +3627,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>93</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>117</v>
       </c>
@@ -3700,7 +3703,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>118</v>
       </c>
@@ -3738,7 +3741,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>64</v>
       </c>
@@ -3776,7 +3779,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>154</v>
       </c>
@@ -3814,7 +3817,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>85</v>
       </c>
@@ -3852,7 +3855,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>172</v>
       </c>
@@ -3890,7 +3893,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>124</v>
       </c>
@@ -3928,7 +3931,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>134</v>
       </c>
@@ -3966,7 +3969,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>115</v>
       </c>
@@ -3998,13 +4001,13 @@
         <v>0</v>
       </c>
       <c r="N55" t="s">
-        <v>176</v>
+        <v>463</v>
       </c>
       <c r="Q55" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>174</v>
       </c>
@@ -4042,7 +4045,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -4080,7 +4083,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>116</v>
       </c>
@@ -4118,7 +4121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4156,7 +4159,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>106</v>
       </c>
@@ -4194,7 +4197,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>104</v>
       </c>
@@ -4232,7 +4235,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>44</v>
       </c>
@@ -4270,7 +4273,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>145</v>
       </c>
@@ -4308,7 +4311,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>7</v>
       </c>
@@ -4346,7 +4349,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>24</v>
       </c>
@@ -4384,7 +4387,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>164</v>
       </c>
@@ -4422,7 +4425,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>18</v>
       </c>
@@ -4460,7 +4463,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>58</v>
       </c>
@@ -4498,7 +4501,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>119</v>
       </c>
@@ -4536,7 +4539,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>98</v>
       </c>
@@ -4574,7 +4577,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>89</v>
       </c>
@@ -4612,7 +4615,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>133</v>
       </c>
@@ -4650,7 +4653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>22</v>
       </c>
@@ -4688,7 +4691,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4726,7 +4729,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>143</v>
       </c>
@@ -4764,7 +4767,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>163</v>
       </c>
@@ -4802,7 +4805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>146</v>
       </c>
@@ -4840,7 +4843,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>41</v>
       </c>
@@ -4878,7 +4881,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>11</v>
       </c>
@@ -4916,7 +4919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>56</v>
       </c>
@@ -4954,7 +4957,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
@@ -4992,7 +4995,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>63</v>
       </c>
@@ -5030,7 +5033,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>103</v>
       </c>
@@ -5068,7 +5071,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>10</v>
       </c>
@@ -5106,7 +5109,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>69</v>
       </c>
@@ -5144,7 +5147,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>20</v>
       </c>
@@ -5182,7 +5185,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>129</v>
       </c>
@@ -5220,7 +5223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>173</v>
       </c>
@@ -5258,7 +5261,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>37</v>
       </c>
@@ -5296,7 +5299,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>149</v>
       </c>
@@ -5334,7 +5337,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>19</v>
       </c>
@@ -5372,7 +5375,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>52</v>
       </c>
@@ -5410,7 +5413,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>108</v>
       </c>
@@ -5448,7 +5451,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>61</v>
       </c>
@@ -5486,7 +5489,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>45</v>
       </c>
@@ -5524,7 +5527,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="96" spans="1:17">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>48</v>
       </c>
@@ -5562,7 +5565,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="97" spans="1:17">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>90</v>
       </c>
@@ -5600,7 +5603,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:17">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>150</v>
       </c>
@@ -5638,7 +5641,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="1:17">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>152</v>
       </c>
@@ -5676,7 +5679,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>60</v>
       </c>
@@ -5714,7 +5717,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="101" spans="1:17">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>165</v>
       </c>
@@ -5752,7 +5755,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>70</v>
       </c>
@@ -5790,7 +5793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:17">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>128</v>
       </c>
@@ -5828,7 +5831,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>111</v>
       </c>
@@ -5866,7 +5869,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="105" spans="1:17">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>28</v>
       </c>
@@ -5904,7 +5907,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>12</v>
       </c>
@@ -5942,7 +5945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>66</v>
       </c>
@@ -5980,7 +5983,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>23</v>
       </c>
@@ -6018,7 +6021,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="109" spans="1:17">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>123</v>
       </c>
@@ -6056,7 +6059,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>159</v>
       </c>
@@ -6094,7 +6097,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:17">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>16</v>
       </c>
@@ -6132,7 +6135,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:17">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>62</v>
       </c>
@@ -6170,7 +6173,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>73</v>
       </c>
@@ -6208,7 +6211,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>40</v>
       </c>
@@ -6246,7 +6249,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>109</v>
       </c>
@@ -6284,7 +6287,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>161</v>
       </c>
@@ -6322,7 +6325,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>67</v>
       </c>
@@ -6360,7 +6363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>102</v>
       </c>
@@ -6398,7 +6401,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>147</v>
       </c>
@@ -6436,7 +6439,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>30</v>
       </c>
@@ -6474,7 +6477,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="121" spans="1:17">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>112</v>
       </c>
@@ -6512,7 +6515,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="122" spans="1:17">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>95</v>
       </c>
@@ -6550,7 +6553,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:17">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>6</v>
       </c>
@@ -6588,7 +6591,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="124" spans="1:17">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>166</v>
       </c>
@@ -6626,7 +6629,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="125" spans="1:17">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>75</v>
       </c>
@@ -6664,7 +6667,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="126" spans="1:17">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>32</v>
       </c>
@@ -6702,7 +6705,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="127" spans="1:17">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>101</v>
       </c>
@@ -6740,7 +6743,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="128" spans="1:17">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>51</v>
       </c>
@@ -6778,7 +6781,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="1:17">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>107</v>
       </c>
@@ -6816,7 +6819,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="130" spans="1:17">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>76</v>
       </c>
@@ -6854,7 +6857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="131" spans="1:17">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>81</v>
       </c>
@@ -6892,7 +6895,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="132" spans="1:17">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>50</v>
       </c>
@@ -6930,7 +6933,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="133" spans="1:17">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>79</v>
       </c>
@@ -6968,7 +6971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="134" spans="1:17">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>94</v>
       </c>
@@ -7006,7 +7009,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="135" spans="1:17">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>34</v>
       </c>
@@ -7044,7 +7047,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="136" spans="1:17">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>97</v>
       </c>
@@ -7082,7 +7085,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="137" spans="1:17">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>36</v>
       </c>
@@ -7120,7 +7123,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="138" spans="1:17">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>171</v>
       </c>
@@ -7158,7 +7161,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="139" spans="1:17">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>141</v>
       </c>
@@ -7196,7 +7199,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="140" spans="1:17">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>114</v>
       </c>
@@ -7234,7 +7237,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>27</v>
       </c>
@@ -7272,7 +7275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:17">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>91</v>
       </c>
@@ -7310,7 +7313,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="143" spans="1:17">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>33</v>
       </c>
@@ -7348,7 +7351,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="144" spans="1:17">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>92</v>
       </c>
@@ -7386,7 +7389,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="145" spans="1:17">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>14</v>
       </c>
@@ -7424,7 +7427,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="146" spans="1:17">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>158</v>
       </c>
@@ -7462,7 +7465,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="147" spans="1:17">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>80</v>
       </c>
@@ -7500,7 +7503,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="148" spans="1:17">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>5</v>
       </c>
@@ -7538,7 +7541,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="149" spans="1:17">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>126</v>
       </c>
@@ -7576,7 +7579,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="150" spans="1:17">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>156</v>
       </c>
@@ -7614,7 +7617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="151" spans="1:17">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>99</v>
       </c>
@@ -7652,7 +7655,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="152" spans="1:17">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>162</v>
       </c>
@@ -7690,7 +7693,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="153" spans="1:17">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>153</v>
       </c>
@@ -7728,7 +7731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="154" spans="1:17">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>155</v>
       </c>
@@ -7766,7 +7769,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="155" spans="1:17">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>17</v>
       </c>
@@ -7804,7 +7807,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="156" spans="1:17">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>144</v>
       </c>
@@ -7842,7 +7845,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="157" spans="1:17">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>148</v>
       </c>
@@ -7880,7 +7883,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="158" spans="1:17">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>46</v>
       </c>
@@ -7918,7 +7921,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="159" spans="1:17">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>122</v>
       </c>
@@ -7956,7 +7959,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="160" spans="1:17">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>87</v>
       </c>
@@ -7994,7 +7997,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="161" spans="1:17">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>84</v>
       </c>
@@ -8032,7 +8035,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="162" spans="1:17">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>39</v>
       </c>
@@ -8070,7 +8073,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="163" spans="1:17">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>136</v>
       </c>
@@ -8108,7 +8111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="164" spans="1:17">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>77</v>
       </c>
@@ -8146,7 +8149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="165" spans="1:17">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>96</v>
       </c>
@@ -8184,7 +8187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="166" spans="1:17">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>68</v>
       </c>
@@ -8222,7 +8225,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="167" spans="1:17">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>21</v>
       </c>
@@ -8260,7 +8263,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="168" spans="1:17">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>9</v>
       </c>
@@ -8298,7 +8301,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="169" spans="1:17">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>71</v>
       </c>
@@ -8336,7 +8339,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="170" spans="1:17">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>55</v>
       </c>
@@ -8374,7 +8377,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="171" spans="1:17">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>157</v>
       </c>
@@ -8412,7 +8415,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="172" spans="1:17">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>131</v>
       </c>
@@ -8450,7 +8453,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="173" spans="1:17">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>86</v>
       </c>
@@ -8504,15 +8507,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010066CBBDD130B1F44A896A70F9AD4F8534" ma:contentTypeVersion="7" ma:contentTypeDescription="Utwórz nowy dokument." ma:contentTypeScope="" ma:versionID="5917357e7ffb9dd7f5ecc8ad0705072e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf55cb2f-1a6a-4287-a545-65627ac8b2ab" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="422a0d09a4306a057e5c944836a4450e" ns2:_="">
     <xsd:import namespace="cf55cb2f-1a6a-4287-a545-65627ac8b2ab"/>
@@ -8674,10 +8668,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3027E159-CF77-40D5-8EB2-CE2571609BE0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C010198B-B937-4A1A-8A3A-054C30222E38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf55cb2f-1a6a-4287-a545-65627ac8b2ab"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C010198B-B937-4A1A-8A3A-054C30222E38}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3027E159-CF77-40D5-8EB2-CE2571609BE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>